<commit_message>
update department not shown up correctly bug
</commit_message>
<xml_diff>
--- a/helper/Capability.xlsx
+++ b/helper/Capability.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="162">
   <si>
     <t>Capability</t>
   </si>
@@ -67,19 +67,31 @@
     <t>COE-HR-EHS</t>
   </si>
   <si>
-    <t>COE-HR-Culture_Development</t>
+    <t>COE-HR-Culture_and_Internal_Communications</t>
   </si>
   <si>
     <t>COE-HR-Organization_Development</t>
   </si>
   <si>
-    <t>COE-HR-Recruiting</t>
-  </si>
-  <si>
-    <t>COE-HR-Salary_Management</t>
-  </si>
-  <si>
-    <t>COE-HR-SSC_Management</t>
+    <t>COE-HR-Learning_Development</t>
+  </si>
+  <si>
+    <t>COE-HR-Talent_Aquisition</t>
+  </si>
+  <si>
+    <t>COE-HR-Total_Rewards</t>
+  </si>
+  <si>
+    <t>COE-HR-HRBP_HQ</t>
+  </si>
+  <si>
+    <t>EB-HR-HRBP_HQ</t>
+  </si>
+  <si>
+    <t>EB-HR-HRBP_Country</t>
+  </si>
+  <si>
+    <t>COE-HR_Employee_Experience_and_Delivery</t>
   </si>
   <si>
     <t>COE-Legal-EU_Legal</t>
@@ -247,7 +259,7 @@
     <t>Emergency_situation_dry_run,Purchasing_standard_for_consumable_products</t>
   </si>
   <si>
-    <t>NIO_Cultural_Workshop_Process</t>
+    <t>NIO_Cultural_Workshop_Process,hr test_process</t>
   </si>
   <si>
     <t>EU_Company_Car_Policy,EU_RSU_Policy,Holiday_Policy,Recruiting_&amp;_Interview_Process,NCP_Policy,Sickness_Leave,Head_Count_Planning,Org_Change_Process</t>
@@ -259,9 +271,6 @@
     <t>Annual_Bonus_Policy,Local_market_Salary_Benchmark</t>
   </si>
   <si>
-    <t>SSC_Development,SSC_Operation</t>
-  </si>
-  <si>
     <t>EU_Contract_template_standard,Contract_review_standard,Legal_Supplier_Selection,EU_legal_dispute_handling_process,System_Requirement_Legal_Review_Process,Privacy Impact Assessment (PIA),Maintenance of Register of Processing Activities (RoPA)</t>
   </si>
   <si>
@@ -298,7 +307,7 @@
     <t>Community_Event_Operation,Community_Event_Planning</t>
   </si>
   <si>
-    <t>Community_Partner_Development,Community_Referral_Program_Development</t>
+    <t>Community_Partner_Development_2_0,Community_Referral_Program_Development</t>
   </si>
   <si>
     <t>Gather Voice of Users Process (VOC)</t>
@@ -328,7 +337,7 @@
     <t>EU_NH_design_and_approval_process,_Design_vendor_pool_selection_process,_EU_NIO_House_Space_Hub_design_guidline,,Budget approval and management process (including change mana),  DOA_and_paymanet_process,  Budget_making_and_rolling_process</t>
   </si>
   <si>
-    <t xml:space="preserve">  Construction management process (including managing vendors),  Construction_vendor_pool_selection_and_management_process,  NH_NS_Nhub_opening_preparation_standard,  NH_NS_Nhub_operation_management_,  EU_POS_Infrastructure_projects_tracking_and_change_management</t>
+    <t>Construction management process (including managing vendors),  Construction_vendor_pool_selection_and_management_process,  NH_NS_Nhub_opening_preparation_standard,  NH_NS_Nhub_operation_management_,  EU_POS_Infrastructure_projects_tracking_and_change_management</t>
   </si>
   <si>
     <t>Daily_NH_Store_Closing_SOP,Daily_NH_Store_Opening_SOP,NIO_House_Purchase_Consumables,NIO_House_Reception_Process,Space_Reservation_Operation,NIO_House_vehicle_information_display_Standard,NIO_House_Property_Insurance_Process,NIO_House_parts_display_standard,NIO_House_NHS_shift_management</t>
@@ -349,7 +358,7 @@
     <t>User_experiences_2D_testdrive coupon,User_orders_Purchase_car,User_Change_of_Ownership,User_Request_Leasing,User_Request_Subscription_cancelation,User_asks_about_car_or_price_or_model_etc_,User_gets_normal_delivery,User_mutually_follows_a_NIO_employee_on_NIO_app,User_orders_Leasing_car,User_orders_Subscription_car,User_orders_something_from_NIO_cafe,User_pays_the_final_payment,User_performs_a_FOTA_upgrade,User_returns_a_leasing_car,User_returns_a_subscription_car,User_subscribes_NIO_newletter,User_wants_to_book_testdrive_online,User_wants_to_cancel_or_modify_NIO_Life_order,Receive_subscription_order_from_user,Deliver_subscription_cars,Subscription_cars_delivery-related,Send_vehicle_preparation_order_to_RDC_and_the_registration_order_to_DAD,User_returns_a_Purchase_car,User_experiences_normal_testdrive ,Fellow_complete_testdrive_process,Fellow_handles_a_testdrive_cancelation_or_change_request,Fellow_manually_books_testdrive_for_user,Fellow_testdrive_car_preparation,Fellow_follows_up_testdrive_leads,Fellow_fills_damage_form_together_with_users,Employee_process_new_purchase_oder,User_Purchase_car_after_delivery,  Leads_classification_and_follow_up_process_management,  Test_Drive_outbound_call_and_communication_Post-test_drive_follow-up_process,Test_drive_site_selection_layout_and_process_design_,_Group_Test_Drive_Process_-_Standardize_the_group_test_drive_process,Fellow_Performance_Evaluation_Process,  Order_and_stock_planning_and_management_Process,Demo_car_and_display_car_management,_Appointment-to-delivery_process,Power_Swap_call_center_handles_user_call,Location_scouting_for_power_swap_station,Fellow_handles_a_Testdrive_Process</t>
   </si>
   <si>
-    <t>_FIFO_steering_and_fleet_management,Fleet_Transport_Management,Fleet_planning_process,2B_system_development_process,test_process</t>
+    <t>_FIFO_steering_and_fleet_management,Fleet_Transport_Management,Fleet_planning_process,2B_system_development_process</t>
   </si>
   <si>
     <t>Sales_Report_Generation_Standard,Intelligence_data_architecture_design_standard,Data_Cleanup_Process,Data_interface_Design_Process</t>
@@ -848,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -882,19 +891,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -905,16 +914,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -925,19 +934,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -948,19 +957,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -971,19 +980,19 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -994,19 +1003,19 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1017,19 +1026,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1040,19 +1049,19 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1063,16 +1072,16 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1083,19 +1092,19 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1106,19 +1115,19 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1129,19 +1138,19 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G13" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1152,19 +1161,19 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1175,19 +1184,10 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
-      </c>
-      <c r="G15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1198,19 +1198,19 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1221,19 +1221,19 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G17" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1244,19 +1244,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1267,19 +1258,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1290,16 +1269,10 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1310,19 +1283,10 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F21" t="s">
         <v>122</v>
-      </c>
-      <c r="G21" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1333,16 +1297,19 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="E22" t="s">
+        <v>85</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1353,16 +1320,19 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1373,16 +1343,16 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1393,13 +1363,19 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" t="s">
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G25" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1410,19 +1386,16 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G26" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1433,19 +1406,16 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1456,19 +1426,16 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G28" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1479,19 +1446,13 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1502,19 +1463,19 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1525,13 +1486,19 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
       </c>
       <c r="G31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1542,19 +1509,19 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
         <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1565,19 +1532,19 @@
         <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
         <v>91</v>
       </c>
       <c r="F33" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1588,19 +1555,19 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E34" t="s">
         <v>92</v>
       </c>
       <c r="F34" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1611,19 +1578,13 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="G35" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1634,19 +1595,19 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G36" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1657,19 +1618,19 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G37" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1680,19 +1641,19 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G38" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1703,19 +1664,19 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G39" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1726,19 +1687,19 @@
         <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G40" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1749,19 +1710,19 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" t="s">
         <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1772,19 +1733,19 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1795,19 +1756,19 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D43" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G43" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1818,19 +1779,19 @@
         <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G44" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1841,19 +1802,19 @@
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G45" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1864,19 +1825,19 @@
         <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1887,19 +1848,19 @@
         <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G47" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1910,19 +1871,19 @@
         <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G48" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1933,19 +1894,19 @@
         <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D49" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G49" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1956,19 +1917,19 @@
         <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" t="s">
         <v>137</v>
       </c>
       <c r="G50" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1979,19 +1940,19 @@
         <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F51" t="s">
         <v>138</v>
       </c>
       <c r="G51" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2002,19 +1963,19 @@
         <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F52" t="s">
         <v>139</v>
       </c>
       <c r="G52" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2025,19 +1986,19 @@
         <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F53" t="s">
         <v>140</v>
       </c>
       <c r="G53" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2048,19 +2009,19 @@
         <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D54" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G54" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2071,19 +2032,19 @@
         <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F55" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G55" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2094,19 +2055,19 @@
         <v>60</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F56" t="s">
         <v>142</v>
       </c>
       <c r="G56" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2117,19 +2078,19 @@
         <v>61</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D57" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F57" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="G57" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2140,13 +2101,19 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="E58" t="s">
+        <v>115</v>
+      </c>
+      <c r="F58" t="s">
+        <v>144</v>
       </c>
       <c r="G58" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2157,13 +2124,19 @@
         <v>63</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="E59" t="s">
+        <v>116</v>
+      </c>
+      <c r="F59" t="s">
+        <v>143</v>
       </c>
       <c r="G59" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2174,13 +2147,93 @@
         <v>64</v>
       </c>
       <c r="C60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="s">
+        <v>117</v>
+      </c>
+      <c r="F60" t="s">
+        <v>145</v>
+      </c>
+      <c r="G60" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
         <v>65</v>
       </c>
-      <c r="D60" t="s">
+      <c r="C61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" t="s">
+        <v>71</v>
+      </c>
+      <c r="E61" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" t="s">
+        <v>129</v>
+      </c>
+      <c r="G61" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
         <v>66</v>
       </c>
-      <c r="G60" t="s">
-        <v>157</v>
+      <c r="C62" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make reference links update
</commit_message>
<xml_diff>
--- a/helper/Capability.xlsx
+++ b/helper/Capability.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="177">
   <si>
     <t>Capability</t>
   </si>
@@ -118,13 +118,13 @@
     <t>COE-Power-LTO</t>
   </si>
   <si>
-    <t>COE-PE-Product_Planning</t>
-  </si>
-  <si>
-    <t>COE-PE-Product_Experience</t>
-  </si>
-  <si>
-    <t>COE-PE-Vehicle_Quality</t>
+    <t>COE-PD-Product_Planning</t>
+  </si>
+  <si>
+    <t>COE-PD-Product_Experience</t>
+  </si>
+  <si>
+    <t>COE-PD-Vehicle_Quality</t>
   </si>
   <si>
     <t>COE-Purchase-Vendor_Management</t>
@@ -208,6 +208,9 @@
     <t>EB-UO-Commercial_Product</t>
   </si>
   <si>
+    <t>EB-UO-Partner_Strategy</t>
+  </si>
+  <si>
     <t>EB-Satisfaction-SCR</t>
   </si>
   <si>
@@ -223,7 +226,7 @@
     <t>EB-UO-Fleet_Planning</t>
   </si>
   <si>
-    <t>LINK</t>
+    <t>Click Me</t>
   </si>
   <si>
     <t>Achieve_Sales_Target</t>
@@ -235,6 +238,9 @@
     <t>EU_Data_Security_Control_Policy,Colleague_Request_New_System_Feature,New_Feature_UI_Approval_Process,European_Feature_Scheduling_Process</t>
   </si>
   <si>
+    <t>ud_publishes_a_pgc</t>
+  </si>
+  <si>
     <t>New_Feature_Release_Process</t>
   </si>
   <si>
@@ -253,6 +259,9 @@
     <t>5_Year_Budget ,Current_Year_Budget_Planning</t>
   </si>
   <si>
+    <t>Example_Finance_Controlling_Process</t>
+  </si>
+  <si>
     <t>Create_Course_Materials,Training_Quality_Evaluation_Process,Event_market_product_Launch_preparation,Operate_Training_Sessions,Product_Launch_Training_Operation,Train_the_Trainer_Operation,Training_Handover_&amp;_Evaluation,eLearning_System_Management</t>
   </si>
   <si>
@@ -265,6 +274,9 @@
     <t>EU_Company_Car_Policy,EU_RSU_Policy,Holiday_Policy,Recruiting_&amp;_Interview_Process,NCP_Policy,Sickness_Leave,Head_Count_Planning,Org_Change_Process</t>
   </si>
   <si>
+    <t>Example_learning_development_Process</t>
+  </si>
+  <si>
     <t>Recruiting_Process,Onboarding_Process</t>
   </si>
   <si>
@@ -280,6 +292,18 @@
     <t>Power_Swap_Operator_helps_user_complete_swap,Power_Swap_call_center_handles_user_call,Power_home_charger_activation_process,Power_related_low_star_follow_up_process,Power_Product_planning_process,Power_Charging_network_partner_Selection,Power_Charging_and_product_Pricing_Standard</t>
   </si>
   <si>
+    <t>Example_Power_R&amp;M</t>
+  </si>
+  <si>
+    <t>Example_Power_Battery_&amp;_Satefy</t>
+  </si>
+  <si>
+    <t>Example_Power_Market_Management</t>
+  </si>
+  <si>
+    <t>Example_Power_LTO_process</t>
+  </si>
+  <si>
     <t>FOTA_Launch_Preparation,FOTA_Operation,New_Model_Go_to_Market_Operation</t>
   </si>
   <si>
@@ -295,6 +319,9 @@
     <t>Standard_Purchase_Process,Emergency_Purchase_Process,Order_Negociation_Process,Contract_Review_Process,Contract_Management,Purchasing_process</t>
   </si>
   <si>
+    <t>Example_GR_Process</t>
+  </si>
+  <si>
     <t>Financial_Offer_Product_Design,NIO_Partner_Management_Process</t>
   </si>
   <si>
@@ -334,7 +361,7 @@
     <t>Network_Development_Dashboard_Report_Standard,  Location_Approval_Process,Network_Location_Planning,Location_Scouting_Process,Scouting_Vendor_Selection_and_management_process</t>
   </si>
   <si>
-    <t>EU_NH_design_and_approval_process,_Design_vendor_pool_selection_process,_EU_NIO_House_Space_Hub_design_guidline,,Budget approval and management process (including change mana),  DOA_and_paymanet_process,  Budget_making_and_rolling_process</t>
+    <t>EU_NH_design_and_approval_process,_Design_vendor_pool_selection_process,_EU_NIO_House_Space_Hub_design_guidline,,Budget approval and management process (including change mana),  DOA_and_paymanet_process,  Budget_making_and_rolling_process,Network_development_manager_selects_design_vendor</t>
   </si>
   <si>
     <t>Construction management process (including managing vendors),  Construction_vendor_pool_selection_and_management_process,  NH_NS_Nhub_opening_preparation_standard,  NH_NS_Nhub_operation_management_,  EU_POS_Infrastructure_projects_tracking_and_change_management</t>
@@ -346,7 +373,7 @@
     <t>NIO_House_Event_operation,Big_Event_planning,NIO_House_Event_planning,Big_Event_operation,Event_Location_Selection,Event_Vendor_Selection,Event_Communication,Event_preparation_&amp;_training</t>
   </si>
   <si>
-    <t>Create_EU_PR_Strategy,Operate_PR_relate_Events,PGC_drafting_standard,OGC_drafting_standard_,Post_event_communication_requirement_,</t>
+    <t>Create_EU_PR_Strategy,Operate_PR_relate_Events,PGC_drafting_standard,OGC_drafting_standard_,Post_event_communication_requirement_2_2,</t>
   </si>
   <si>
     <t>Public_Conference_Organization,Public_Crisis_Management_Process,Plan_PR_related_Events,Publish_PR_PGC_&amp;_Press_Release</t>
@@ -355,7 +382,7 @@
     <t>2B_Product_Development,2B_Client_Strategy,asdasdsad</t>
   </si>
   <si>
-    <t>User_experiences_2D_testdrive coupon,User_orders_Purchase_car,User_Change_of_Ownership,User_Request_Leasing,User_Request_Subscription_cancelation,User_asks_about_car_or_price_or_model_etc_,User_gets_normal_delivery,User_mutually_follows_a_NIO_employee_on_NIO_app,User_orders_Leasing_car,User_orders_Subscription_car,User_orders_something_from_NIO_cafe,User_pays_the_final_payment,User_performs_a_FOTA_upgrade,User_returns_a_leasing_car,User_returns_a_subscription_car,User_subscribes_NIO_newletter,User_wants_to_book_testdrive_online,User_wants_to_cancel_or_modify_NIO_Life_order,Receive_subscription_order_from_user,Deliver_subscription_cars,Subscription_cars_delivery-related,Send_vehicle_preparation_order_to_RDC_and_the_registration_order_to_DAD,User_returns_a_Purchase_car,User_experiences_normal_testdrive ,Fellow_complete_testdrive_process,Fellow_handles_a_testdrive_cancelation_or_change_request,Fellow_manually_books_testdrive_for_user,Fellow_testdrive_car_preparation,Fellow_follows_up_testdrive_leads,Fellow_fills_damage_form_together_with_users,Employee_process_new_purchase_oder,User_Purchase_car_after_delivery,  Leads_classification_and_follow_up_process_management,  Test_Drive_outbound_call_and_communication_Post-test_drive_follow-up_process,Test_drive_site_selection_layout_and_process_design_,_Group_Test_Drive_Process_-_Standardize_the_group_test_drive_process,Fellow_Performance_Evaluation_Process,  Order_and_stock_planning_and_management_Process,Demo_car_and_display_car_management,_Appointment-to-delivery_process,Power_Swap_call_center_handles_user_call,Location_scouting_for_power_swap_station,Fellow_handles_a_Testdrive_Process</t>
+    <t>User_experiences_2D_testdrive coupon,User_orders_Purchase_car,User_Change_of_Ownership,User_Request_Leasing,User_Request_Subscription_cancelation,User_asks_about_car_or_price_or_model_etc_,User_gets_normal_delivery,User_mutually_follows_a_NIO_employee_on_NIO_app,User_orders_Leasing_car,User_orders_Subscription_car,User_orders_something_from_NIO_cafe,User_pays_the_final_payment,User_performs_a_FOTA_upgrade,User_returns_a_leasing_car,User_returns_a_subscription_car,User_subscribes_NIO_newletter,User_wants_to_book_testdrive_online,User_wants_to_cancel_or_modify_NIO_Life_order,Receive_subscription_order_from_user,Deliver_subscription_cars,Subscription_cars_delivery-related,Send_vehicle_preparation_order_to_RDC_and_the_registration_order_to_DAD,User_returns_a_Purchase_car,User_experiences_normal_testdrive ,Fellow_complete_testdrive_process,Fellow_handles_a_testdrive_cancelation_or_change_request,Fellow_manually_books_testdrive_for_user,Fellow_testdrive_car_preparation,Fellow_follows_up_testdrive_leads,Fellow_fills_damage_form_together_with_users,Employee_process_new_purchase_oder,User_Purchase_car_after_delivery,  Leads_classification_and_follow_up_process_management,  Test_Drive_outbound_call_and_communication_Post-test_drive_follow-up_process,Test_drive_site_selection_layout_and_process_design_,_Group_Test_Drive_Process_-_Standardize_the_group_test_drive_process,Fellow_Performance_Evaluation_Process,  Order_and_stock_planning_and_management_Process,Demo_car_and_display_car_management,_Appointment-to-delivery_process,Power_Swap_call_center_handles_user_call,Location_scouting_for_power_swap_station,Fellow_handles_a_Testdrive_Process,Fellow_test_drive_follow_up_sop</t>
   </si>
   <si>
     <t>_FIFO_steering_and_fleet_management,Fleet_Transport_Management,Fleet_planning_process,2B_system_development_process</t>
@@ -367,12 +394,24 @@
     <t>Subscription_Product_Planning,Used_Car_Planning,Commercial_product_pricing,Market_Scan_&amp;_Analysis,RV_Management,Purchase_Product_planning,Financial_Leasing_product_planning</t>
   </si>
   <si>
+    <t>partner_Strategy_development_process</t>
+  </si>
+  <si>
     <t>Agent_Performance_Review,SCR_-_SOP_-_Activate_Home_Charger,SCR_-_SOP_-_Answers_Debug,SCR_-_SOP_-_Buy_a_car,SCR_-_SOP_-_Cancel_Testdrive,SCR_-_SOP_-_Handles_Low_Star,SCR_-_SOP_-_Rebook_Testdrive,SCR_-_SOP_-_Test_Drive_Request,SCR_-_SOP_-_User_Account_Deletion,SCR_-_SOP_-_Validate_UGC,SCR_Complaint_Handling,SCR_FAQ_Update,SCR_Onboarding_Training,SCR_Shift_Management,SCR_Vendor_Payment,SCR_Wiki_Management,User_asks_SCR_due_to_power_problem,User_contacts_SCR_to_delete_NIO_account,SCR_receives_One-click_service_booking_request_from_subscription_user,SCR_receives_One-click_service_cancel_request_from_subscription_user,NIO_SCR_receives_RSA_request,SCR_handles_One-click_service_</t>
   </si>
   <si>
     <t>Emergency_Handling_Process,Mysterious_AmbassadorOpen_Check_process_and_standard_,Small_loop-closing,_Big_loop-closing,Establish_EU_user_complaint_escalation_and_response_mechanism_,Low_star_follow_Up_Process,Weekly_Satisfaction_Report_Standard</t>
   </si>
   <si>
+    <t>5_Year_Sales_Planning</t>
+  </si>
+  <si>
+    <t>5_Year_Production_Plannign</t>
+  </si>
+  <si>
+    <t>Current_year_Fleet_Planning</t>
+  </si>
+  <si>
     <t>Digital_Development_PMO_Team</t>
   </si>
   <si>
@@ -388,16 +427,19 @@
     <t>Legal_EU_Department</t>
   </si>
   <si>
-    <t>NIO_Life</t>
-  </si>
-  <si>
-    <t>Power Market_Launch &amp; Enabling Team</t>
-  </si>
-  <si>
-    <t>Product Marketing Department (PMK)</t>
-  </si>
-  <si>
-    <t>Operational_Procurement</t>
+    <t>NIO_Life_Supply_Chain_Department</t>
+  </si>
+  <si>
+    <t>Power_market_launch_and_enabling_team</t>
+  </si>
+  <si>
+    <t>Product_Marketing_Department</t>
+  </si>
+  <si>
+    <t>Europe_Product_Experience_Department</t>
+  </si>
+  <si>
+    <t>Purchasing_Governance_and_BP_Team</t>
   </si>
   <si>
     <t>Business_Development</t>
@@ -415,10 +457,10 @@
     <t>Service_Planning_Team</t>
   </si>
   <si>
-    <t>Operation_Support</t>
-  </si>
-  <si>
-    <t>Parts_&amp;_Logistics</t>
+    <t>Operation_Support,Service_PMO</t>
+  </si>
+  <si>
+    <t>Parts_and_Logistics</t>
   </si>
   <si>
     <t>Network_Development</t>
@@ -436,10 +478,10 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Communication_&amp;_PR</t>
-  </si>
-  <si>
-    <t>Fleet_&amp;_Business_Sales</t>
+    <t>Communication_and_PR</t>
+  </si>
+  <si>
+    <t>Fleet_and_Business_Sales</t>
   </si>
   <si>
     <t>Retail_Sales</t>
@@ -451,6 +493,9 @@
     <t>Business_Intelligence</t>
   </si>
   <si>
+    <t>Partner_Strategy</t>
+  </si>
+  <si>
     <t>Service_Coordinator</t>
   </si>
   <si>
@@ -469,7 +514,7 @@
     <t>COE_Legal</t>
   </si>
   <si>
-    <t>COE NIO_Life</t>
+    <t>COE_NIO_Life</t>
   </si>
   <si>
     <t>COE Power_Operation</t>
@@ -857,7 +902,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -891,19 +936,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -914,16 +959,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G3" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -934,19 +982,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -957,19 +1005,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G5" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -980,19 +1028,19 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="G6" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1003,19 +1051,19 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1026,19 +1074,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1049,19 +1097,19 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="G9" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1072,16 +1120,19 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1092,19 +1143,19 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1115,19 +1166,19 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1138,19 +1189,19 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G13" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1161,19 +1212,19 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G14" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1184,10 +1235,19 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>135</v>
+      </c>
+      <c r="G15" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1198,19 +1258,19 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G16" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1221,19 +1281,19 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G17" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1244,10 +1304,16 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>122</v>
+        <v>135</v>
+      </c>
+      <c r="G18" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1258,7 +1324,13 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1269,10 +1341,16 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>135</v>
+      </c>
+      <c r="G20" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1283,10 +1361,16 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>135</v>
+      </c>
+      <c r="G21" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1297,19 +1381,19 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="G22" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1320,19 +1404,19 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="G23" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1343,16 +1427,16 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="G24" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1363,19 +1447,19 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G25" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1386,16 +1470,19 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G26" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1406,16 +1493,19 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
       </c>
       <c r="F27" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G27" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1426,16 +1516,19 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G28" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1446,13 +1539,19 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" t="s">
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G29" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1463,19 +1562,19 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="G30" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1486,19 +1585,19 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F31" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="G31" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1509,42 +1608,27 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="G32" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
       <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" t="s">
-        <v>91</v>
-      </c>
-      <c r="F33" t="s">
-        <v>127</v>
-      </c>
-      <c r="G33" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1552,22 +1636,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F34" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="G34" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1575,16 +1659,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>141</v>
       </c>
       <c r="G35" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1592,22 +1682,19 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="G36" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1615,22 +1702,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="G37" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1638,22 +1725,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D38" t="s">
         <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F38" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="G38" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1661,22 +1748,22 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E39" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F39" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="G39" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1684,22 +1771,22 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E40" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F40" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="G40" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1707,22 +1794,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E41" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F41" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="G41" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1730,22 +1817,22 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F42" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="G42" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1753,22 +1840,22 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F43" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="G43" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1776,22 +1863,22 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1799,22 +1886,22 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F45" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="G45" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1822,22 +1909,22 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E46" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="G46" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1845,22 +1932,22 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G47" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1868,22 +1955,22 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="G48" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1891,22 +1978,22 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
         <v>71</v>
       </c>
       <c r="E49" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F49" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="G49" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1914,22 +2001,22 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F50" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="G50" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1937,22 +2024,22 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="F51" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="G51" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1960,22 +2047,22 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D52" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F52" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="G52" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1983,22 +2070,22 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E53" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F53" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="G53" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2006,22 +2093,22 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E54" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F54" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="G54" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2029,22 +2116,22 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E55" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="G55" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2052,22 +2139,22 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="F56" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="G56" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2075,22 +2162,22 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F57" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2098,22 +2185,22 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E58" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F58" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="G58" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2121,22 +2208,22 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E59" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F59" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="G59" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2144,22 +2231,22 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
         <v>71</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F60" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="G60" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2167,22 +2254,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
         <v>71</v>
       </c>
       <c r="E61" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F61" t="s">
-        <v>129</v>
-      </c>
-      <c r="G61" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2190,16 +2274,22 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="E62" t="s">
+        <v>127</v>
+      </c>
+      <c r="F62" t="s">
+        <v>160</v>
       </c>
       <c r="G62" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2207,16 +2297,22 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="E63" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" t="s">
+        <v>143</v>
       </c>
       <c r="G63" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2224,16 +2320,59 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" t="s">
+        <v>71</v>
+      </c>
+      <c r="E64" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
         <v>68</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" t="s">
+        <v>130</v>
+      </c>
+      <c r="G65" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
         <v>69</v>
       </c>
-      <c r="D64" t="s">
-        <v>70</v>
-      </c>
-      <c r="G64" t="s">
-        <v>160</v>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" t="s">
+        <v>131</v>
+      </c>
+      <c r="G66" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>